<commit_message>
Solution to Exercise 3 Chapter 5
Solution to Exercise 3 Chapter 5
</commit_message>
<xml_diff>
--- a/Exercises/FactorRequCapitalV.xlsx
+++ b/Exercises/FactorRequCapitalV.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenri\Google Drive\Cosas del trabajo\SAS\SASUniversityEdition\myfolders\aar\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3C1E7D-C151-48BD-86B4-9F3F0413E235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C75EAC-11C5-458F-B6AD-A85364079953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F16673F-F143-4FC2-91CF-6169E7B9A107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$217</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,12 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="66">
-  <si>
-    <t>Meses 
-vencido
- s r</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="14">
   <si>
     <t>Madurez (meses)</t>
   </si>
@@ -50,84 +48,6 @@
     <t>m&gt;60</t>
   </si>
   <si>
-    <t>m&gt;61</t>
-  </si>
-  <si>
-    <t>m&gt;62</t>
-  </si>
-  <si>
-    <t>m&gt;63</t>
-  </si>
-  <si>
-    <t>m&gt;64</t>
-  </si>
-  <si>
-    <t>m&gt;65</t>
-  </si>
-  <si>
-    <t>m&gt;66</t>
-  </si>
-  <si>
-    <t>m&gt;67</t>
-  </si>
-  <si>
-    <t>m&gt;68</t>
-  </si>
-  <si>
-    <t>m&gt;69</t>
-  </si>
-  <si>
-    <t>m&gt;70</t>
-  </si>
-  <si>
-    <t>m&gt;71</t>
-  </si>
-  <si>
-    <t>m&gt;72</t>
-  </si>
-  <si>
-    <t>m&gt;73</t>
-  </si>
-  <si>
-    <t>m&gt;74</t>
-  </si>
-  <si>
-    <t>m&gt;75</t>
-  </si>
-  <si>
-    <t>m&gt;76</t>
-  </si>
-  <si>
-    <t>m&gt;77</t>
-  </si>
-  <si>
-    <t>m&gt;78</t>
-  </si>
-  <si>
-    <t>m&gt;79</t>
-  </si>
-  <si>
-    <t>m&gt;80</t>
-  </si>
-  <si>
-    <t>m&gt;81</t>
-  </si>
-  <si>
-    <t>m&gt;82</t>
-  </si>
-  <si>
-    <t>m&gt;83</t>
-  </si>
-  <si>
-    <t>m&gt;84</t>
-  </si>
-  <si>
-    <t>m&gt;85</t>
-  </si>
-  <si>
-    <t>m&gt;86</t>
-  </si>
-  <si>
     <t>l &gt; 88.4057%</t>
   </si>
   <si>
@@ -140,91 +60,16 @@
     <t>V</t>
   </si>
   <si>
-    <t>m≤60</t>
+    <t>No Pesos</t>
   </si>
   <si>
-    <t>m≤61</t>
+    <t>Meses vencido</t>
   </si>
   <si>
-    <t>m≤62</t>
+    <t>m&lt;=60</t>
   </si>
   <si>
-    <t>m≤63</t>
-  </si>
-  <si>
-    <t>m≤64</t>
-  </si>
-  <si>
-    <t>m≤65</t>
-  </si>
-  <si>
-    <t>m≤66</t>
-  </si>
-  <si>
-    <t>m≤67</t>
-  </si>
-  <si>
-    <t>m≤68</t>
-  </si>
-  <si>
-    <t>m≤69</t>
-  </si>
-  <si>
-    <t>m≤70</t>
-  </si>
-  <si>
-    <t>m≤71</t>
-  </si>
-  <si>
-    <t>m≤72</t>
-  </si>
-  <si>
-    <t>m≤73</t>
-  </si>
-  <si>
-    <t>m≤74</t>
-  </si>
-  <si>
-    <t>m≤75</t>
-  </si>
-  <si>
-    <t>m≤76</t>
-  </si>
-  <si>
-    <t>m≤77</t>
-  </si>
-  <si>
-    <t>m≤78</t>
-  </si>
-  <si>
-    <t>m≤79</t>
-  </si>
-  <si>
-    <t>m≤80</t>
-  </si>
-  <si>
-    <t>m≤81</t>
-  </si>
-  <si>
-    <t>m≤82</t>
-  </si>
-  <si>
-    <t>m≤83</t>
-  </si>
-  <si>
-    <t>m≤84</t>
-  </si>
-  <si>
-    <t>m≤85</t>
-  </si>
-  <si>
-    <t>m≤86</t>
-  </si>
-  <si>
-    <t>l ≤ 88.4057%</t>
-  </si>
-  <si>
-    <t>No Pesos</t>
+    <t>l &lt;= 88.4057%</t>
   </si>
 </sst>
 </file>
@@ -584,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA7AA16-88B7-458B-A7F8-02173F840502}">
   <dimension ref="A1:F217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B221" sqref="B221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,22 +445,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -623,16 +468,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>3.3000000000000002E-2</v>
@@ -643,16 +488,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>3.9100000000000003E-2</v>
@@ -663,16 +508,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>6.8500000000000005E-2</v>
@@ -683,16 +528,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>0.1101</v>
@@ -703,16 +548,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>0.1759</v>
@@ -723,16 +568,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>0.20280000000000001</v>
@@ -743,16 +588,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>0.23630000000000001</v>
@@ -763,16 +608,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>0.26590000000000003</v>
@@ -783,16 +628,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>0.29559999999999997</v>
@@ -803,16 +648,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>0.3241</v>
@@ -823,16 +668,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>0.35709999999999997</v>
@@ -843,16 +688,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>0.39</v>
@@ -863,16 +708,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>0.43059999999999998</v>
@@ -883,16 +728,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>0.46850000000000003</v>
@@ -903,16 +748,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>0.50729999999999997</v>
@@ -923,16 +768,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>0.55000000000000004</v>
@@ -943,16 +788,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>0.58799999999999997</v>
@@ -963,16 +808,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <v>0.63249999999999995</v>
@@ -983,16 +828,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>0.69450000000000001</v>
@@ -1003,16 +848,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>0.74019999999999997</v>
@@ -1023,16 +868,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>0.78690000000000004</v>
@@ -1043,16 +888,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F23">
         <v>0.86870000000000003</v>
@@ -1063,16 +908,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <v>0.96160000000000001</v>
@@ -1083,16 +928,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1103,16 +948,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1123,16 +968,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1140,19 +985,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1163,16 +1008,16 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F29">
         <v>9.4600000000000004E-2</v>
@@ -1183,16 +1028,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F30">
         <v>0.1047</v>
@@ -1203,16 +1048,16 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F31">
         <v>0.13700000000000001</v>
@@ -1223,16 +1068,16 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F32">
         <v>0.17230000000000001</v>
@@ -1243,16 +1088,16 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F33">
         <v>0.4229</v>
@@ -1263,16 +1108,16 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F34">
         <v>0.44230000000000003</v>
@@ -1283,16 +1128,16 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F35">
         <v>0.4753</v>
@@ -1303,16 +1148,16 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F36">
         <v>0.50609999999999999</v>
@@ -1323,16 +1168,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F37">
         <v>0.53420000000000001</v>
@@ -1343,16 +1188,16 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F38">
         <v>0.56020000000000003</v>
@@ -1363,16 +1208,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F39">
         <v>0.58760000000000001</v>
@@ -1383,16 +1228,16 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F40">
         <v>0.61309999999999998</v>
@@ -1403,16 +1248,16 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F41">
         <v>0.63900000000000001</v>
@@ -1423,16 +1268,16 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <v>0.71419999999999995</v>
@@ -1443,16 +1288,16 @@
         <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <v>0.73409999999999997</v>
@@ -1463,16 +1308,16 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F44">
         <v>0.754</v>
@@ -1483,16 +1328,16 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <v>0.77249999999999996</v>
@@ -1503,16 +1348,16 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F46">
         <v>0.79379999999999995</v>
@@ -1523,16 +1368,16 @@
         <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F47">
         <v>0.8155</v>
@@ -1543,16 +1388,16 @@
         <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F48">
         <v>0.70750000000000002</v>
@@ -1563,16 +1408,16 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F49">
         <v>0.86109999999999998</v>
@@ -1583,16 +1428,16 @@
         <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F50">
         <v>0.89539999999999997</v>
@@ -1603,16 +1448,16 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F51">
         <v>0.92379999999999995</v>
@@ -1623,16 +1468,16 @@
         <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F52">
         <v>0.95209999999999995</v>
@@ -1643,16 +1488,16 @@
         <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F53">
         <v>0.97799999999999998</v>
@@ -1663,16 +1508,16 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F54">
         <v>0.99929999999999997</v>
@@ -1680,19 +1525,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -1703,16 +1548,16 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F56">
         <v>6.8999999999999999E-3</v>
@@ -1723,16 +1568,16 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F57">
         <v>1.04E-2</v>
@@ -1743,16 +1588,16 @@
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F58">
         <v>2.24E-2</v>
@@ -1763,16 +1608,16 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F59">
         <v>3.78E-2</v>
@@ -1783,16 +1628,16 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F60">
         <v>9.4100000000000003E-2</v>
@@ -1803,16 +1648,16 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F61">
         <v>0.1087</v>
@@ -1823,16 +1668,16 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F62">
         <v>0.1303</v>
@@ -1843,16 +1688,16 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F63">
         <v>0.15049999999999999</v>
@@ -1863,16 +1708,16 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F64">
         <v>0.17460000000000001</v>
@@ -1883,16 +1728,16 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F65">
         <v>0.19550000000000001</v>
@@ -1903,16 +1748,16 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F66">
         <v>0.2218</v>
@@ -1923,16 +1768,16 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F67">
         <v>0.24560000000000001</v>
@@ -1943,16 +1788,16 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D68" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F68">
         <v>0.27210000000000001</v>
@@ -1963,16 +1808,16 @@
         <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F69">
         <v>0.36969999999999997</v>
@@ -1983,16 +1828,16 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F70">
         <v>0.40570000000000001</v>
@@ -2003,16 +1848,16 @@
         <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F71">
         <v>0.4541</v>
@@ -2023,16 +1868,16 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E72" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F72">
         <v>0.50560000000000005</v>
@@ -2043,16 +1888,16 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F73">
         <v>0.94520000000000004</v>
@@ -2063,16 +1908,16 @@
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D74" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F74">
         <v>0.60219999999999996</v>
@@ -2083,16 +1928,16 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D75" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F75">
         <v>0.68589999999999995</v>
@@ -2103,16 +1948,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D76" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F76">
         <v>0.72499999999999998</v>
@@ -2123,16 +1968,16 @@
         <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D77" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F77">
         <v>0.79769999999999996</v>
@@ -2143,16 +1988,16 @@
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F78">
         <v>0.88539999999999996</v>
@@ -2163,16 +2008,16 @@
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E79" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -2183,16 +2028,16 @@
         <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2203,16 +2048,16 @@
         <v>25</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D81" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E81" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2220,19 +2065,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D82" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E82" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2243,16 +2088,16 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E83" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F83">
         <v>1.04E-2</v>
@@ -2263,16 +2108,16 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D84" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F84">
         <v>1.37E-2</v>
@@ -2283,16 +2128,16 @@
         <v>2</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D85" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F85">
         <v>2.5399999999999999E-2</v>
@@ -2303,16 +2148,16 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D86" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F86">
         <v>3.9E-2</v>
@@ -2323,16 +2168,16 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D87" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F87">
         <v>0.14760000000000001</v>
@@ -2343,16 +2188,16 @@
         <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F88">
         <v>0.16070000000000001</v>
@@ -2363,16 +2208,16 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F89">
         <v>0.1789</v>
@@ -2383,16 +2228,16 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D90" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F90">
         <v>0.19850000000000001</v>
@@ -2403,16 +2248,16 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E91" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F91">
         <v>0.2162</v>
@@ -2423,16 +2268,16 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D92" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E92" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F92">
         <v>0.2344</v>
@@ -2443,16 +2288,16 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D93" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E93" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F93">
         <v>0.2525</v>
@@ -2463,16 +2308,16 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D94" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E94" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F94">
         <v>0.2666</v>
@@ -2483,16 +2328,16 @@
         <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F95">
         <v>0.27989999999999998</v>
@@ -2503,16 +2348,16 @@
         <v>13</v>
       </c>
       <c r="B96" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E96" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F96">
         <v>0.45069999999999999</v>
@@ -2523,16 +2368,16 @@
         <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E97" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F97">
         <v>0.46810000000000002</v>
@@ -2543,16 +2388,16 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D98" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F98">
         <v>0.4879</v>
@@ -2563,16 +2408,16 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D99" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E99" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F99">
         <v>0.50880000000000003</v>
@@ -2583,16 +2428,16 @@
         <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D100" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E100" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F100">
         <v>0.52829999999999999</v>
@@ -2603,16 +2448,16 @@
         <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D101" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F101">
         <v>0.55320000000000003</v>
@@ -2623,16 +2468,16 @@
         <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D102" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E102" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F102">
         <v>0.57620000000000005</v>
@@ -2643,16 +2488,16 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E103" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F103">
         <v>0.60270000000000001</v>
@@ -2663,16 +2508,16 @@
         <v>21</v>
       </c>
       <c r="B104" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D104" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F104">
         <v>0.62760000000000005</v>
@@ -2683,16 +2528,16 @@
         <v>22</v>
       </c>
       <c r="B105" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E105" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F105">
         <v>0.65159999999999996</v>
@@ -2703,16 +2548,16 @@
         <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D106" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F106">
         <v>0.68600000000000005</v>
@@ -2723,16 +2568,16 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D107" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E107" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F107">
         <v>0.70199999999999996</v>
@@ -2743,16 +2588,16 @@
         <v>25</v>
       </c>
       <c r="B108" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D108" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E108" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F108">
         <v>0.72850000000000004</v>
@@ -2760,19 +2605,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E109" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -2783,16 +2628,16 @@
         <v>0</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E110" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F110">
         <v>9.9299999999999999E-2</v>
@@ -2803,16 +2648,16 @@
         <v>1</v>
       </c>
       <c r="B111" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E111" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F111">
         <v>0.1119</v>
@@ -2823,16 +2668,16 @@
         <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E112" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F112">
         <v>0.1578</v>
@@ -2843,16 +2688,16 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E113" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F113">
         <v>0.20219999999999999</v>
@@ -2863,16 +2708,16 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F114">
         <v>0.25869999999999999</v>
@@ -2883,16 +2728,16 @@
         <v>5</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F115">
         <v>0.27529999999999999</v>
@@ -2903,16 +2748,16 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E116" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F116">
         <v>0.30549999999999999</v>
@@ -2923,16 +2768,16 @@
         <v>7</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F117">
         <v>0.33379999999999999</v>
@@ -2943,16 +2788,16 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E118" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F118">
         <v>0.35970000000000002</v>
@@ -2963,16 +2808,16 @@
         <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E119" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F119">
         <v>0.38750000000000001</v>
@@ -2983,16 +2828,16 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E120" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F120">
         <v>0.41760000000000003</v>
@@ -3003,16 +2848,16 @@
         <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E121" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F121">
         <v>0.4456</v>
@@ -3023,16 +2868,16 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F122">
         <v>0.47449999999999998</v>
@@ -3043,16 +2888,16 @@
         <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E123" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F123">
         <v>0.49669999999999997</v>
@@ -3063,16 +2908,16 @@
         <v>14</v>
       </c>
       <c r="B124" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E124" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F124">
         <v>0.52749999999999997</v>
@@ -3083,16 +2928,16 @@
         <v>15</v>
       </c>
       <c r="B125" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E125" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F125">
         <v>0.56330000000000002</v>
@@ -3103,16 +2948,16 @@
         <v>16</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E126" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F126">
         <v>0.59919999999999995</v>
@@ -3123,16 +2968,16 @@
         <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E127" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F127">
         <v>0.64080000000000004</v>
@@ -3143,16 +2988,16 @@
         <v>18</v>
       </c>
       <c r="B128" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E128" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F128">
         <v>0.68520000000000003</v>
@@ -3163,16 +3008,16 @@
         <v>19</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F129">
         <v>0.72570000000000001</v>
@@ -3183,16 +3028,16 @@
         <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E130" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F130">
         <v>0.76359999999999995</v>
@@ -3203,16 +3048,16 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E131" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F131">
         <v>0.81689999999999996</v>
@@ -3223,16 +3068,16 @@
         <v>22</v>
       </c>
       <c r="B132" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E132" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F132">
         <v>0.86609999999999998</v>
@@ -3243,16 +3088,16 @@
         <v>23</v>
       </c>
       <c r="B133" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E133" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F133">
         <v>0.92459999999999998</v>
@@ -3263,16 +3108,16 @@
         <v>24</v>
       </c>
       <c r="B134" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E134" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F134">
         <v>0.97199999999999998</v>
@@ -3283,16 +3128,16 @@
         <v>25</v>
       </c>
       <c r="B135" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E135" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -3300,19 +3145,19 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -3323,16 +3168,16 @@
         <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C137" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E137" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F137">
         <v>0.155</v>
@@ -3343,16 +3188,16 @@
         <v>1</v>
       </c>
       <c r="B138" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C138" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E138" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F138">
         <v>0.16259999999999999</v>
@@ -3363,16 +3208,16 @@
         <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C139" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E139" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F139">
         <v>0.18690000000000001</v>
@@ -3383,16 +3228,16 @@
         <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C140" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D140" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E140" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F140">
         <v>0.22239999999999999</v>
@@ -3403,16 +3248,16 @@
         <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C141" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D141" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E141" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F141">
         <v>0.37640000000000001</v>
@@ -3423,16 +3268,16 @@
         <v>5</v>
       </c>
       <c r="B142" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C142" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D142" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E142" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F142">
         <v>0.40510000000000002</v>
@@ -3443,16 +3288,16 @@
         <v>6</v>
       </c>
       <c r="B143" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C143" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D143" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E143" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F143">
         <v>0.43859999999999999</v>
@@ -3463,16 +3308,16 @@
         <v>7</v>
       </c>
       <c r="B144" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C144" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E144" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F144">
         <v>0.47049999999999997</v>
@@ -3483,16 +3328,16 @@
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C145" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D145" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E145" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F145">
         <v>0.50349999999999995</v>
@@ -3503,16 +3348,16 @@
         <v>9</v>
       </c>
       <c r="B146" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C146" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D146" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E146" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F146">
         <v>0.5373</v>
@@ -3523,16 +3368,16 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C147" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D147" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E147" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F147">
         <v>0.56810000000000005</v>
@@ -3543,16 +3388,16 @@
         <v>11</v>
       </c>
       <c r="B148" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D148" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E148" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F148">
         <v>0.59309999999999996</v>
@@ -3563,16 +3408,16 @@
         <v>12</v>
       </c>
       <c r="B149" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C149" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D149" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E149" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F149">
         <v>0.61880000000000002</v>
@@ -3583,16 +3428,16 @@
         <v>13</v>
       </c>
       <c r="B150" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C150" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D150" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E150" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F150">
         <v>0.67779999999999996</v>
@@ -3603,16 +3448,16 @@
         <v>14</v>
       </c>
       <c r="B151" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C151" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D151" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E151" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F151">
         <v>0.70550000000000002</v>
@@ -3623,16 +3468,16 @@
         <v>15</v>
       </c>
       <c r="B152" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C152" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D152" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E152" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F152">
         <v>0.73089999999999999</v>
@@ -3643,16 +3488,16 @@
         <v>16</v>
       </c>
       <c r="B153" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C153" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D153" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E153" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F153">
         <v>0.75819999999999999</v>
@@ -3663,16 +3508,16 @@
         <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C154" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D154" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E154" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F154">
         <v>0.7903</v>
@@ -3683,16 +3528,16 @@
         <v>18</v>
       </c>
       <c r="B155" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C155" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D155" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E155" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F155">
         <v>0.82110000000000005</v>
@@ -3703,16 +3548,16 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C156" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E156" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F156">
         <v>0.85419999999999996</v>
@@ -3723,16 +3568,16 @@
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D157" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E157" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F157">
         <v>0.88660000000000005</v>
@@ -3743,16 +3588,16 @@
         <v>21</v>
       </c>
       <c r="B158" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C158" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D158" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E158" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F158">
         <v>0.92179999999999995</v>
@@ -3763,16 +3608,16 @@
         <v>22</v>
       </c>
       <c r="B159" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C159" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D159" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E159" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F159">
         <v>0.95340000000000003</v>
@@ -3783,16 +3628,16 @@
         <v>23</v>
       </c>
       <c r="B160" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C160" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D160" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E160" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F160">
         <v>0.97729999999999995</v>
@@ -3803,16 +3648,16 @@
         <v>24</v>
       </c>
       <c r="B161" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D161" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E161" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F161">
         <v>1</v>
@@ -3823,16 +3668,16 @@
         <v>25</v>
       </c>
       <c r="B162" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C162" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D162" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E162" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F162">
         <v>1</v>
@@ -3840,19 +3685,19 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B163" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D163" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E163" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F163">
         <v>1</v>
@@ -3863,16 +3708,16 @@
         <v>0</v>
       </c>
       <c r="B164" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D164" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E164" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F164">
         <v>1.1299999999999999E-2</v>
@@ -3883,16 +3728,16 @@
         <v>1</v>
       </c>
       <c r="B165" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D165" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E165" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F165">
         <v>1.47E-2</v>
@@ -3903,16 +3748,16 @@
         <v>2</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D166" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E166" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F166">
         <v>2.5499999999999998E-2</v>
@@ -3923,16 +3768,16 @@
         <v>3</v>
       </c>
       <c r="B167" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D167" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E167" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F167">
         <v>3.5400000000000001E-2</v>
@@ -3943,16 +3788,16 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E168" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F168">
         <v>7.9000000000000001E-2</v>
@@ -3963,16 +3808,16 @@
         <v>5</v>
       </c>
       <c r="B169" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D169" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E169" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F169">
         <v>8.5000000000000006E-2</v>
@@ -3983,16 +3828,16 @@
         <v>6</v>
       </c>
       <c r="B170" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D170" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E170" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F170">
         <v>9.7900000000000001E-2</v>
@@ -4003,16 +3848,16 @@
         <v>7</v>
       </c>
       <c r="B171" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D171" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E171" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F171">
         <v>0.10829999999999999</v>
@@ -4023,16 +3868,16 @@
         <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D172" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E172" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F172">
         <v>0.1201</v>
@@ -4043,16 +3888,16 @@
         <v>9</v>
       </c>
       <c r="B173" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D173" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F173">
         <v>0.13039999999999999</v>
@@ -4063,16 +3908,16 @@
         <v>10</v>
       </c>
       <c r="B174" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D174" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E174" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F174">
         <v>0.14249999999999999</v>
@@ -4083,16 +3928,16 @@
         <v>11</v>
       </c>
       <c r="B175" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D175" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E175" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F175">
         <v>0.15670000000000001</v>
@@ -4103,16 +3948,16 @@
         <v>12</v>
       </c>
       <c r="B176" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D176" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E176" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F176">
         <v>0.17069999999999999</v>
@@ -4123,16 +3968,16 @@
         <v>13</v>
       </c>
       <c r="B177" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D177" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E177" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F177">
         <v>0.2089</v>
@@ -4143,16 +3988,16 @@
         <v>14</v>
       </c>
       <c r="B178" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D178" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E178" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F178">
         <v>0.22689999999999999</v>
@@ -4163,16 +4008,16 @@
         <v>15</v>
       </c>
       <c r="B179" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D179" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E179" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F179">
         <v>0.2457</v>
@@ -4183,16 +4028,16 @@
         <v>16</v>
       </c>
       <c r="B180" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D180" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E180" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F180">
         <v>0.26740000000000003</v>
@@ -4203,16 +4048,16 @@
         <v>17</v>
       </c>
       <c r="B181" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D181" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E181" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F181">
         <v>0.2893</v>
@@ -4223,16 +4068,16 @@
         <v>18</v>
       </c>
       <c r="B182" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D182" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E182" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F182">
         <v>0.31690000000000002</v>
@@ -4243,16 +4088,16 @@
         <v>19</v>
       </c>
       <c r="B183" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D183" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E183" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F183">
         <v>0.33960000000000001</v>
@@ -4263,16 +4108,16 @@
         <v>20</v>
       </c>
       <c r="B184" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D184" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E184" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F184">
         <v>0.36320000000000002</v>
@@ -4283,16 +4128,16 @@
         <v>21</v>
       </c>
       <c r="B185" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D185" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E185" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F185">
         <v>0.3926</v>
@@ -4303,16 +4148,16 @@
         <v>22</v>
       </c>
       <c r="B186" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D186" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E186" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F186">
         <v>0.4224</v>
@@ -4323,16 +4168,16 @@
         <v>23</v>
       </c>
       <c r="B187" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D187" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E187" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F187">
         <v>0.45179999999999998</v>
@@ -4343,16 +4188,16 @@
         <v>24</v>
       </c>
       <c r="B188" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D188" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E188" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F188">
         <v>0.48709999999999998</v>
@@ -4363,16 +4208,16 @@
         <v>25</v>
       </c>
       <c r="B189" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D189" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E189" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F189">
         <v>0.53859999999999997</v>
@@ -4380,19 +4225,19 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C190" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E190" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F190">
         <v>1</v>
@@ -4403,16 +4248,16 @@
         <v>0</v>
       </c>
       <c r="B191" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C191" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E191" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F191">
         <v>1.9400000000000001E-2</v>
@@ -4423,16 +4268,16 @@
         <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C192" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E192" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F192">
         <v>2.12E-2</v>
@@ -4443,16 +4288,16 @@
         <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C193" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D193" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E193" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F193">
         <v>2.7E-2</v>
@@ -4463,16 +4308,16 @@
         <v>3</v>
       </c>
       <c r="B194" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C194" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D194" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E194" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F194">
         <v>3.4299999999999997E-2</v>
@@ -4483,16 +4328,16 @@
         <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C195" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D195" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E195" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F195">
         <v>0.1694</v>
@@ -4503,16 +4348,16 @@
         <v>5</v>
       </c>
       <c r="B196" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C196" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D196" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E196" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F196">
         <v>0.18140000000000001</v>
@@ -4523,16 +4368,16 @@
         <v>6</v>
       </c>
       <c r="B197" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C197" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D197" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E197" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F197">
         <v>0.1968</v>
@@ -4543,16 +4388,16 @@
         <v>7</v>
       </c>
       <c r="B198" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C198" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D198" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E198" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F198">
         <v>0.2122</v>
@@ -4563,16 +4408,16 @@
         <v>8</v>
       </c>
       <c r="B199" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C199" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D199" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E199" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F199">
         <v>0.2276</v>
@@ -4583,16 +4428,16 @@
         <v>9</v>
       </c>
       <c r="B200" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C200" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D200" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E200" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F200">
         <v>0.24249999999999999</v>
@@ -4603,16 +4448,16 @@
         <v>10</v>
       </c>
       <c r="B201" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C201" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D201" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E201" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F201">
         <v>0.25790000000000002</v>
@@ -4623,16 +4468,16 @@
         <v>11</v>
       </c>
       <c r="B202" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C202" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D202" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E202" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F202">
         <v>0.27350000000000002</v>
@@ -4643,16 +4488,16 @@
         <v>12</v>
       </c>
       <c r="B203" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C203" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D203" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E203" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F203">
         <v>0.2903</v>
@@ -4663,16 +4508,16 @@
         <v>13</v>
       </c>
       <c r="B204" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C204" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D204" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E204" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F204">
         <v>0.38900000000000001</v>
@@ -4683,16 +4528,16 @@
         <v>14</v>
       </c>
       <c r="B205" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C205" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D205" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E205" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F205">
         <v>0.40789999999999998</v>
@@ -4703,16 +4548,16 @@
         <v>15</v>
       </c>
       <c r="B206" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C206" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D206" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E206" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F206">
         <v>0.42459999999999998</v>
@@ -4723,16 +4568,16 @@
         <v>16</v>
       </c>
       <c r="B207" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C207" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D207" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E207" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F207">
         <v>0.4446</v>
@@ -4743,16 +4588,16 @@
         <v>17</v>
       </c>
       <c r="B208" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C208" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D208" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E208" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F208">
         <v>0.46379999999999999</v>
@@ -4763,16 +4608,16 @@
         <v>18</v>
       </c>
       <c r="B209" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C209" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D209" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E209" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F209">
         <v>0.48530000000000001</v>
@@ -4783,16 +4628,16 @@
         <v>19</v>
       </c>
       <c r="B210" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C210" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D210" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E210" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F210">
         <v>0.50929999999999997</v>
@@ -4803,16 +4648,16 @@
         <v>20</v>
       </c>
       <c r="B211" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C211" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D211" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E211" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F211">
         <v>0.53010000000000002</v>
@@ -4823,16 +4668,16 @@
         <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C212" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D212" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E212" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F212">
         <v>0.55059999999999998</v>
@@ -4843,16 +4688,16 @@
         <v>22</v>
       </c>
       <c r="B213" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C213" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D213" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E213" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F213">
         <v>0.57189999999999996</v>
@@ -4863,16 +4708,16 @@
         <v>23</v>
       </c>
       <c r="B214" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C214" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D214" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E214" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F214">
         <v>0.59030000000000005</v>
@@ -4883,16 +4728,16 @@
         <v>24</v>
       </c>
       <c r="B215" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C215" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D215" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E215" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F215">
         <v>0.61099999999999999</v>
@@ -4903,16 +4748,16 @@
         <v>25</v>
       </c>
       <c r="B216" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C216" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D216" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E216" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F216">
         <v>0.62649999999999995</v>
@@ -4920,25 +4765,26 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C217" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="D217" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E217" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F217">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F217" xr:uid="{CBA77130-8950-4208-8E18-39416DCCB1E1}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>